<commit_message>
fixed loggers of main.py and scraper.py, rotation of user agents, ordering HTTP headers
</commit_message>
<xml_diff>
--- a/exported-files/products.xlsx
+++ b/exported-files/products.xlsx
@@ -61,7 +61,7 @@
     <t>Fantom P 1200 Pratic Kırmızı Kuru Süpürge</t>
   </si>
   <si>
-    <t>396.00</t>
+    <t>415.36</t>
   </si>
   <si>
     <t>https://productimages.hepsiburada.net/s/31/550/10341451530290.jpg</t>
@@ -73,7 +73,7 @@
     <t>4.6</t>
   </si>
   <si>
-    <t>4389</t>
+    <t>4393</t>
   </si>
 </sst>
 </file>

</xml_diff>